<commit_message>
Alteração na documentação de Plano de Riscos
</commit_message>
<xml_diff>
--- a/docs/PlanoDeRiscos.xlsx
+++ b/docs/PlanoDeRiscos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="When">[1]Param!$I$5:$I$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>Responsável</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Entrar em contato com membros da equipe sobre tarefas pendentes</t>
   </si>
   <si>
-    <t xml:space="preserve">Realizar monitoriais semanais com o membro </t>
-  </si>
-  <si>
     <t>Conversa motivacional; Acompanhamento mais próximo</t>
   </si>
   <si>
@@ -216,15 +213,6 @@
     <t>Fazer reuniões semanais; Utilizar ferramentas de comunicação de fácil acesso por toda a equipe</t>
   </si>
   <si>
-    <t xml:space="preserve">Consultar Biblioteca; Consultar professores; Frequentar monitoria </t>
-  </si>
-  <si>
-    <t>Verificar disponibilidade antes do início do projeto; Manter horário de reunião</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consultar ata da reunião; Conversar com membro da equipe </t>
-  </si>
-  <si>
     <t>Repositório; Ambiente de trabalho de fácil configuração</t>
   </si>
   <si>
@@ -232,6 +220,12 @@
   </si>
   <si>
     <t xml:space="preserve">Participar de assembleias de alunos  manisfestando motivação contra a greve </t>
+  </si>
+  <si>
+    <t>Alinhar com o membro faltoso individualmente após a reunião, assim que possível</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar disponibilidade antes do início do projeto; Manter horário de reunião; Conversar com membro da equipe  </t>
   </si>
 </sst>
 </file>
@@ -778,7 +772,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,7 +807,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1069,7 +1063,7 @@
         <v>42882</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -1500,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1541,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>50</v>
@@ -1558,7 +1552,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>51</v>
@@ -1569,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>52</v>
@@ -1580,7 +1574,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>49</v>
@@ -1591,7 +1585,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>53</v>
@@ -1602,7 +1596,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>54</v>
@@ -1613,7 +1607,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>55</v>
@@ -1624,36 +1618,25 @@
         <v>30</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>

</xml_diff>